<commit_message>
Sauce Changes + Test Cases
Added Top Menubar
Log in, Logout, Contact us, Visit Us, Sign up For Discount, Create New
Account
</commit_message>
<xml_diff>
--- a/output/com/baublebar/data/TestCases.xlsx
+++ b/output/com/baublebar/data/TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25007"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
   <si>
     <t>TCID</t>
   </si>
@@ -63,6 +63,36 @@
   </si>
   <si>
     <t>DiscountEmail</t>
+  </si>
+  <si>
+    <t>LoadBaublebarTest</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>LoginTest</t>
+  </si>
+  <si>
+    <t>qa@baublebar.com</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>ContactusTest</t>
+  </si>
+  <si>
+    <t>LogoutTest</t>
+  </si>
+  <si>
+    <t>VisitusTest</t>
+  </si>
+  <si>
+    <t>automation</t>
+  </si>
+  <si>
+    <t>ShoppingCartTest</t>
   </si>
 </sst>
 </file>
@@ -99,7 +129,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,7 +144,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.249977111117893"/>
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -143,7 +179,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
@@ -151,20 +187,34 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -458,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -482,16 +532,17 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -499,14 +550,63 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -517,10 +617,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -538,40 +638,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
-        <v>8</v>
+      <c r="A1" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="6" t="s">
-        <v>6</v>
+      <c r="A5" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -581,13 +672,10 @@
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="6" t="s">
-        <v>7</v>
+      <c r="A9" s="8" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -595,10 +683,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -606,17 +694,136 @@
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C31" s="6" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B11" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B11" r:id="rId1" display="cmaitri@yahoo.com"/>
+    <hyperlink ref="B31" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId3"/>
+    <hyperlink ref="B15" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>

</xml_diff>

<commit_message>
Modifies assert for main nav
Modifies assert for main navigation bar because the page change very
frequently causing the test cases to fail. So now asserting on url
</commit_message>
<xml_diff>
--- a/output/com/baublebar/data/TestCases.xlsx
+++ b/output/com/baublebar/data/TestCases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="46">
   <si>
     <t>TCID</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>SubCategoryName</t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>What</t>
   </si>
 </sst>
 </file>
@@ -711,10 +717,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:XFD47"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -986,7 +992,7 @@
         <v>3</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C47" s="12"/>
     </row>
@@ -995,7 +1001,7 @@
         <v>3</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C48" s="12"/>
     </row>
@@ -1004,7 +1010,7 @@
         <v>3</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C49" s="12"/>
     </row>
@@ -1013,7 +1019,7 @@
         <v>3</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C50" s="12"/>
     </row>
@@ -1021,16 +1027,17 @@
       <c r="A51" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="B51" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" s="12"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1038,7 +1045,7 @@
         <v>3</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1046,40 +1053,39 @@
         <v>3</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="14" t="s">
+    <row r="57" spans="1:3">
+      <c r="A57" s="14" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="12"/>
+        <v>41</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C59" s="12"/>
     </row>
@@ -1088,7 +1094,7 @@
         <v>3</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C60" s="12"/>
     </row>
@@ -1097,7 +1103,7 @@
         <v>3</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C61" s="12"/>
     </row>
@@ -1106,7 +1112,7 @@
         <v>3</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C62" s="12"/>
     </row>
@@ -1114,16 +1120,17 @@
       <c r="A63" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="B63" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C63" s="12"/>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1131,7 +1138,7 @@
         <v>3</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1139,6 +1146,14 @@
         <v>3</v>
       </c>
       <c r="B66" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
trying to run using jar files
</commit_message>
<xml_diff>
--- a/output/com/baublebar/data/TestCases.xlsx
+++ b/output/com/baublebar/data/TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25007"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="27100" windowHeight="15820" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="27100" windowHeight="15820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="70">
   <si>
     <t>TCID</t>
   </si>
@@ -119,9 +119,6 @@
     <t>MainNavigationBarTest</t>
   </si>
   <si>
-    <t>What’s New</t>
-  </si>
-  <si>
     <t>Necklaces</t>
   </si>
   <si>
@@ -179,9 +176,6 @@
     <t>FirstName</t>
   </si>
   <si>
-    <t xml:space="preserve">LastName </t>
-  </si>
-  <si>
     <t>City</t>
   </si>
   <si>
@@ -209,17 +203,44 @@
     <t>Dallas</t>
   </si>
   <si>
-    <t>TX</t>
-  </si>
-  <si>
     <t>Street</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>100-100-1000</t>
+  </si>
+  <si>
+    <t>7890</t>
+  </si>
+  <si>
+    <t>CreditCard</t>
+  </si>
+  <si>
+    <t>CVVNumber</t>
+  </si>
+  <si>
+    <t>378282246310005</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>Whats New</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="00000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +275,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -327,7 +354,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -343,6 +370,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -766,7 +798,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
@@ -774,7 +806,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -782,7 +814,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -801,10 +833,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K74"/>
+  <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -815,10 +847,13 @@
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="8" width="12.5" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
     <col min="9" max="9" width="5.6640625" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="15" customWidth="1"/>
     <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1067,7 +1102,7 @@
         <v>2</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C46" s="12"/>
     </row>
@@ -1076,7 +1111,7 @@
         <v>3</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="C47" s="12"/>
     </row>
@@ -1085,7 +1120,7 @@
         <v>3</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C48" s="12"/>
     </row>
@@ -1094,7 +1129,7 @@
         <v>3</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C49" s="12"/>
     </row>
@@ -1103,7 +1138,7 @@
         <v>3</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C50" s="12"/>
     </row>
@@ -1112,7 +1147,7 @@
         <v>3</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C51" s="12"/>
     </row>
@@ -1121,7 +1156,7 @@
         <v>3</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1129,7 +1164,7 @@
         <v>3</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1137,12 +1172,12 @@
         <v>3</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1150,10 +1185,10 @@
         <v>2</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1161,7 +1196,7 @@
         <v>3</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C58" s="12"/>
     </row>
@@ -1170,7 +1205,7 @@
         <v>3</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C59" s="12"/>
     </row>
@@ -1179,7 +1214,7 @@
         <v>3</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C60" s="12"/>
     </row>
@@ -1188,7 +1223,7 @@
         <v>3</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C61" s="12"/>
     </row>
@@ -1197,7 +1232,7 @@
         <v>3</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C62" s="12"/>
     </row>
@@ -1206,7 +1241,7 @@
         <v>3</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1214,119 +1249,131 @@
         <v>3</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
       <c r="A65" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
+      <c r="A66" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
-      <c r="A66" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:13">
       <c r="A68" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
       <c r="A69" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C69" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D69" t="s">
         <v>5</v>
       </c>
       <c r="E69" t="s">
+        <v>50</v>
+      </c>
+      <c r="F69" t="s">
+        <v>61</v>
+      </c>
+      <c r="G69" t="s">
+        <v>60</v>
+      </c>
+      <c r="H69" t="s">
         <v>51</v>
       </c>
-      <c r="F69" t="s">
+      <c r="I69" t="s">
         <v>52</v>
       </c>
-      <c r="G69" t="s">
-        <v>63</v>
-      </c>
-      <c r="H69" t="s">
+      <c r="J69" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="I69" t="s">
+      <c r="K69" t="s">
         <v>54</v>
       </c>
-      <c r="J69" t="s">
+      <c r="L69" t="s">
+        <v>65</v>
+      </c>
+      <c r="M69" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="17">
+      <c r="A70" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C70" t="s">
         <v>55</v>
-      </c>
-      <c r="K69" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11">
-      <c r="A70" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C70" t="s">
-        <v>57</v>
       </c>
       <c r="D70" t="s">
         <v>18</v>
       </c>
       <c r="E70" t="s">
+        <v>56</v>
+      </c>
+      <c r="F70" t="s">
+        <v>57</v>
+      </c>
+      <c r="G70" t="s">
         <v>58</v>
       </c>
-      <c r="F70" t="s">
+      <c r="H70" t="s">
         <v>59</v>
-      </c>
-      <c r="G70" t="s">
-        <v>60</v>
-      </c>
-      <c r="H70" t="s">
-        <v>61</v>
       </c>
       <c r="I70" t="s">
         <v>62</v>
       </c>
-      <c r="J70">
-        <v>7890</v>
-      </c>
-      <c r="K70">
-        <v>1001001000</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11">
+      <c r="J70" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="K70" t="s">
+        <v>63</v>
+      </c>
+      <c r="L70" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="M70" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
       <c r="A72" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
       <c r="A73" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B73" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13">
+      <c r="A74" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11">
-      <c r="A74" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>